<commit_message>
Worked on checking data presence. Next step is to make this a source code
</commit_message>
<xml_diff>
--- a/docs/g2-moderators.xlsx
+++ b/docs/g2-moderators.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Research\FSW\Research_data\JG\SanneG\ICITOP IPD_MA\icitop\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA9AAE5-7CDA-4BB2-9A3F-E62C1E871970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14EBB79-42E0-47A9-99B1-93819330B7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1728" windowWidth="21600" windowHeight="11328" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,20 +28,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>generation</t>
   </si>
   <si>
-    <t>inc</t>
-  </si>
-  <si>
     <t>occ</t>
   </si>
   <si>
-    <t>target</t>
-  </si>
-  <si>
     <t>age</t>
   </si>
   <si>
@@ -51,23 +48,71 @@
     <t>g3</t>
   </si>
   <si>
-    <t>c1</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
     <t>name_construct</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>rst</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>res</t>
+  </si>
+  <si>
+    <t>req</t>
+  </si>
+  <si>
+    <t>vinc</t>
+  </si>
+  <si>
+    <t>edu</t>
+  </si>
+  <si>
+    <t>ses</t>
+  </si>
+  <si>
+    <t>alc</t>
+  </si>
+  <si>
+    <t>dru</t>
+  </si>
+  <si>
+    <t>inv</t>
+  </si>
+  <si>
+    <t>sub</t>
+  </si>
+  <si>
+    <t>nch</t>
+  </si>
+  <si>
+    <t>bir</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,75 +420,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>